<commit_message>
Fix Excel template parsing and add PBMC validation test
</commit_message>
<xml_diff>
--- a/manifests/pbmc/pbmc.xlsx
+++ b/manifests/pbmc/pbmc.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/manifests/pbmc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662A5F9-B3A4-CC49-A7E9-AC6F928B69B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24020" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -279,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0">
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -305,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -318,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -331,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0">
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0">
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -357,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -370,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0">
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -383,12 +389,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="L22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -396,12 +402,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -409,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="0">
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -422,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O22" authorId="0">
+    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -435,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P22" authorId="0">
+    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q22" authorId="0">
+    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -461,7 +467,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0">
+    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -474,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S22" authorId="0">
+    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -487,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T22" authorId="0">
+    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -500,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0">
+    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -513,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0">
+    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -526,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W22" authorId="0">
+    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -539,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0">
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -552,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0">
+    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -565,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0">
+    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -578,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0">
+    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -591,7 +597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB22" authorId="0">
+    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -609,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="70">
   <si>
     <t>#t</t>
   </si>
@@ -762,13 +768,70 @@
   </si>
   <si>
     <t>SAMPLE_STATUS</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Assay-1</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>USPS</t>
+  </si>
+  <si>
+    <t>Frozen (Dry Ice)</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>dfsd</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sdsfd</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Endoscopic Biopsy</t>
+  </si>
+  <si>
+    <t>Unstained Slide</t>
+  </si>
+  <si>
+    <t>dfgd</t>
+  </si>
+  <si>
+    <t>Usable for Assay</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Sample Exhausted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -777,18 +840,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -855,17 +924,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,6 +946,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -919,7 +1000,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,9 +1032,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,6 +1084,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1160,1778 +1277,1897 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-    </row>
-    <row r="2" spans="1:28">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+    </row>
+    <row r="2" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:28">
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-    </row>
-    <row r="6" spans="1:28">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-    </row>
-    <row r="8" spans="1:28">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-    </row>
-    <row r="9" spans="1:28">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-    </row>
-    <row r="11" spans="1:28">
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-    </row>
-    <row r="12" spans="1:28">
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-    </row>
-    <row r="13" spans="1:28">
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-    </row>
-    <row r="14" spans="1:28">
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-    </row>
-    <row r="15" spans="1:28">
+      <c r="C14" s="3">
+        <v>41071</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-    </row>
-    <row r="16" spans="1:28">
+      <c r="C15" s="1">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-    </row>
-    <row r="17" spans="1:28">
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="17" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-    </row>
-    <row r="18" spans="1:28">
+      <c r="C17" s="1">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+    </row>
+    <row r="18" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-    </row>
-    <row r="19" spans="1:28">
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-    </row>
-    <row r="21" spans="1:28">
-      <c r="B21" s="2" t="s">
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="4" t="s">
+      <c r="P22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="T22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U22" s="4" t="s">
+      <c r="U22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V22" s="4" t="s">
+      <c r="V22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="W22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="X22" s="4" t="s">
+      <c r="X22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y22" s="4" t="s">
+      <c r="Y22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Z22" s="4" t="s">
+      <c r="Z22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AA22" s="4" t="s">
+      <c r="AA22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB22" s="4" t="s">
+      <c r="AB22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:28">
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="4">
+        <v>41071</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0.42518518518518517</v>
+      </c>
+      <c r="L23" s="4">
+        <v>41072</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0.42518518518518517</v>
+      </c>
+      <c r="N23" t="s">
+        <v>63</v>
+      </c>
+      <c r="O23" t="s">
+        <v>64</v>
+      </c>
+      <c r="P23" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23">
+        <v>6</v>
+      </c>
+      <c r="S23">
+        <v>6</v>
+      </c>
+      <c r="T23">
+        <v>6</v>
+      </c>
+      <c r="U23">
+        <v>66</v>
+      </c>
+      <c r="V23" t="s">
+        <v>66</v>
+      </c>
+      <c r="W23">
+        <v>12364</v>
+      </c>
+      <c r="X23">
+        <v>123456</v>
+      </c>
+      <c r="Y23">
+        <v>2222</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>24</v>
       </c>
@@ -2942,46 +3178,39 @@
     <mergeCell ref="B21:U21"/>
     <mergeCell ref="V21:AB21"/>
   </mergeCells>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{57FB12A2-839C-CC4C-A3D3-5C791107F4DC}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{385EFECA-5858-044E-A2AF-4CE9B8381A6C}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D924FAAB-EB74-7A4E-AD6B-54788632B6D0}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J23:J222">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J23:J222 L23:L222" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K23:K222">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K23:K222 M23:M222" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
-      <formula2>0.9993055555555556</formula2>
+      <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222">
-      <formula1>AND(ISNUMBER(L23:L222),LEFT(CELL("format",L23:L222),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222">
-      <formula1>0</formula1>
-      <formula2>0.9993055555555556</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Other,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>